<commit_message>
Volledig programma + excel files.
</commit_message>
<xml_diff>
--- a/ControversialResults.xlsx
+++ b/ControversialResults.xlsx
@@ -387,149 +387,421 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://www.thuisarts.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.allesoverseks.be', 'https://www.gezondheidsnet.nl']</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://www.ce.nl', 'https://www.climategate.nl', 'https://www.urgenda.nl', 'https://www.knaw.nl', 'https://www.lne.be']</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.ad.nl', 'https://www.nrc.nl', 'https://www.trouw.nl', 'https://www.omroepbrabant.nl', 'https://www.rtlnieuws.nl', 'https://www.volkskrant.nl', 'https://www.volkskrant.nl', 'houvanarnhem.nl', 'https://www.ed.nl']</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.scientias.nl', 'https://www.umcutrecht.nl', 'https://www.volkskrant.nl', 'https://www.volkskrant.nl', 'https://www.thuisvaccinatie.nl', 'https://www.nrc.nl']</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.parool.nl', 'https://www.volkskrant.nl', 'https://www.volkskrant.nl', 'https://www.amerika.nl', 'https://www.europa-nu.nl', 'https://www.socialevraagstukken.nl', 'ind.nl', 'https://www.trouw.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.gezondheidsnet.nl', 'https://www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://www.urgenda.nl', 'https://www.climategate.nl', 'https://milieudefensie.nl', 'https://www.knaw.nl']</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.lc.nl', 'https://www.nu.nl', 'https://nos.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nrc.nl', 'https://www.omroepbrabant.nl', 'https://www.destentor.nl']</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.umcutrecht.nl', 'https://www.volkskrant.nl', 'https://www.thuisvaccinatie.nl', 'https://www.scientias.nl', 'https://www.nrc.nl', 'https://dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.volkskrant.nl', 'https://www.politie.nl', 'https://europadecentraal.nl', 'https://www.amnesty.nl', 'https://decorrespondent.nl', 'https://www.rijksoverheid.nl', 'https://jalta.nl', 'https://www.socialevraagstukken.nl', 'https://www.europa-nu.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.gezondheidsplein.nl', 'https://www.trouw.nl', 'https://www.thuisarts.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl', 'https://www.ad.nl']</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>['https://www.wur.nl', 'https://www.rijksoverheid.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://www.ce.nl', 'https://www.knaw.nl', 'https://www.climategate.nl', 'https://www.urgenda.nl', 'https://milieudefensie.nl']</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nu.nl', 'https://www.lc.nl', 'https://nos.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nrc.nl', 'https://www.omroepbrabant.nl', 'https://www.destentor.nl']</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.volkskrant.nl', 'https://www.thuisvaccinatie.nl', 'https://www.nrc.nl', 'https://www.scientias.nl', 'https://www.umcutrecht.nl', 'https://mens-en-gezondheid.infonu.nl']</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.volkskrant.nl', 'https://www.amnesty.nl', 'https://europadecentraal.nl', 'https://jalta.nl', 'https://decorrespondent.nl', 'https://www.rijksoverheid.nl', 'https://www.socialevraagstukken.nl', 'https://www.europa-nu.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.gezondheidsnet.nl', 'https://www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://www.urgenda.nl', 'https://www.climategate.nl', 'https://milieudefensie.nl', 'https://www.knaw.nl']</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.lc.nl', 'https://www.nu.nl', 'https://nos.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nrc.nl', 'https://www.omroepbrabant.nl']</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.umcutrecht.nl', 'https://www.thuisvaccinatie.nl', 'https://www.volkskrant.nl', 'https://www.scientias.nl', 'https://dekennisvannu.nl', 'https://www.nrc.nl']</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.volkskrant.nl', 'https://www.politie.nl', 'https://europadecentraal.nl', 'https://www.amnesty.nl', 'https://www.rijksoverheid.nl', 'https://decorrespondent.nl', 'https://jalta.nl', 'https://www.socialevraagstukken.nl', 'https://www.europa-nu.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.gezondheidsplein.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.allesoverseks.be', 'https://www.allesoverseks.be']</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>['https://www.wur.nl', 'https://www.rijksoverheid.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://www.ce.nl', 'https://www.knaw.nl', 'https://www.climategate.nl', 'https://www.urgenda.nl', 'https://www.lne.be']</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nu.nl', 'https://www.lc.nl', 'https://nos.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nrc.nl', 'https://www.omroepbrabant.nl', 'https://joop.bnnvara.nl']</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.volkskrant.nl', 'https://www.scientias.nl', 'https://www.nrc.nl', 'https://www.umcutrecht.nl', 'https://mens-en-gezondheid.infonu.nl']</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.volkskrant.nl', 'https://www.amnesty.nl', 'https://jalta.nl', 'https://europadecentraal.nl', 'https://decorrespondent.nl', 'https://www.rijksoverheid.nl', 'https://www.socialevraagstukken.nl', 'https://www.europa-nu.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.gezondheidsnet.nl', 'https://www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://www.urgenda.nl', 'https://www.climategate.nl', 'https://milieudefensie.nl', 'https://www.knaw.nl']</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nu.nl', 'https://www.lc.nl', 'https://nos.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nrc.nl', 'https://www.omroepbrabant.nl']</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.umcutrecht.nl', 'https://www.thuisvaccinatie.nl', 'https://www.volkskrant.nl', 'https://www.nrc.nl', 'https://www.scientias.nl', 'https://dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.volkskrant.nl', 'https://www.politie.nl', 'https://europadecentraal.nl', 'https://www.amnesty.nl', 'https://www.rijksoverheid.nl', 'https://jalta.nl', 'https://decorrespondent.nl', 'https://www.socialevraagstukken.nl', 'https://www.europa-nu.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.gezondheidsnet.nl', 'https://www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://www.urgenda.nl', 'https://www.climategate.nl', 'https://www.climategate.nl', 'https://milieudefensie.nl']</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nu.nl', 'https://www.lc.nl', 'https://nos.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nrc.nl', 'https://www.omroepbrabant.nl']</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.umcutrecht.nl', 'https://www.volkskrant.nl', 'https://www.nrc.nl', 'https://www.nieuwetijds-kindercoach.nl', 'https://www.rivm.nl']</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.volkskrant.nl', 'https://www.politie.nl', 'https://europadecentraal.nl', 'https://www.amnesty.nl', 'https://jalta.nl', 'https://decorrespondent.nl', 'https://www.rijksoverheid.nl', 'https://www.socialevraagstukken.nl', 'https://www.europa-nu.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>['https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.gezondheidsnet.nl', 'https://www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://www.urgenda.nl', 'https://www.climategate.nl', 'https://milieudefensie.nl', 'https://www.knaw.nl']</t>
+        </is>
+      </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nu.nl', 'https://www.lc.nl', 'https://nos.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nrc.nl']</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.umcutrecht.nl', 'https://www.volkskrant.nl', 'https://www.thuisvaccinatie.nl', 'https://www.scientias.nl', 'https://www.nrc.nl', 'https://dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.volkskrant.nl', 'https://www.politie.nl', 'https://europadecentraal.nl', 'https://www.amnesty.nl', 'https://www.rijksoverheid.nl', 'https://jalta.nl', 'https://decorrespondent.nl', 'https://www.socialevraagstukken.nl', 'https://www.europa-nu.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl/www.rijksoverheid.nl', 'https://www.bloemenhove.nl/www.bloemenhove.nl', 'https://www.bloemenhove.nl/www.bloemenhove.nl', 'https://www.thuisarts.nl/www.thuisarts.nl', 'https://www.trouw.nl/www.trouw.nl', 'https://www.gezondheidsplein.nl/www.gezondheidsplein.nl', 'https://fiom.nl/fiom.nl', 'https://www.telegraaf.nl/www.telegraaf.nl', 'https://www.gezondheidsnet.nl/www.gezondheidsnet.nl', 'https://www.schreeuwomleven.nl/www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl/www.rijksoverheid.nl', 'https://www.wur.nl/www.wur.nl', 'https://www.ce.nl/www.ce.nl', 'https://ec.europa.eu/ec.europa.eu', 'https://www.klimaat.be/www.klimaat.be', 'https://www.hier.nu/www.hier.nu', 'https://www.urgenda.nl/www.urgenda.nl', 'https://www.climategate.nl/www.climategate.nl', 'https://milieudefensie.nl/milieudefensie.nl', 'https://www.knaw.nl/www.knaw.nl']</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl/www.ad.nl', 'https://www.volkskrant.nl/www.volkskrant.nl', 'https://www.trouw.nl/www.trouw.nl', 'https://www.nu.nl/www.nu.nl', 'https://www.lc.nl/www.lc.nl', 'https://nos.nl/nos.nl', 'https://eenvandaag.avrotros.nl/eenvandaag.avrotros.nl', 'https://www.nrc.nl/www.nrc.nl', 'https://www.omroepbrabant.nl/www.omroepbrabant.nl']</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr">
         <is>
           <t>['https://rijksvaccinatieprogramma.nl/rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl/www.nvkp.nl', 'https://www.wanttoknow.nl/www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://stichtingvaccinvrij.nl/stichtingvaccinvrij.nl', 'https://www.umcutrecht.nl/www.umcutrecht.nl', 'https://www.thuisvaccinatie.nl/www.thuisvaccinatie.nl', 'https://www.volkskrant.nl/www.volkskrant.nl', 'https://www.scientias.nl/www.scientias.nl', 'https://dekennisvannu.nl/dekennisvannu.nl', 'https://www.nrc.nl/www.nrc.nl']</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org/nl.wikipedia.org', 'https://www.volkskrant.nl/www.volkskrant.nl', 'https://www.politie.nl/www.politie.nl', 'https://europadecentraal.nl/europadecentraal.nl', 'https://www.amnesty.nl/www.amnesty.nl', 'https://decorrespondent.nl/decorrespondent.nl', 'https://www.rijksoverheid.nl/www.rijksoverheid.nl', 'https://jalta.nl/jalta.nl', 'https://www.socialevraagstukken.nl/www.socialevraagstukken.nl', 'https://www.europa-nu.nl/www.europa-nu.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.schreeuwomleven.nl', 'https://www.gezondheidsnet.nl']</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://www.urgenda.nl', 'https://www.climategate.nl', 'https://milieudefensie.nl', 'https://www.knaw.nl']</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nu.nl', 'https://www.lc.nl', 'https://nos.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nrc.nl', 'https://www.omroepbrabant.nl']</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.umcutrecht.nl', 'https://www.volkskrant.nl', 'https://www.scientias.nl', 'https://www.nrc.nl', 'https://dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.volkskrant.nl', 'https://www.politie.nl', 'https://europadecentraal.nl', 'https://www.amnesty.nl', 'https://decorrespondent.nl', 'https://www.rijksoverheid.nl', 'https://jalta.nl', 'https://www.europa-nu.nl', 'https://www.socialevraagstukken.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl', 'https://www.gezondheidsnet.nl']</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://www.urgenda.nl', 'https://www.climategate.nl', 'https://milieudefensie.nl', 'https://www.knaw.nl']</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nu.nl', 'https://www.lc.nl', 'https://nos.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nrc.nl', 'https://www.omroepbrabant.nl']</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.umcutrecht.nl', 'https://www.volkskrant.nl', 'https://www.nrc.nl', 'https://www.scientias.nl', 'https://dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.volkskrant.nl', 'https://www.politie.nl', 'https://europadecentraal.nl', 'https://www.amnesty.nl', 'https://jalta.nl', 'https://www.rijksoverheid.nl', 'https://decorrespondent.nl', 'https://www.socialevraagstukken.nl', 'https://www.europa-nu.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://www.thuisarts.nl', 'https://fiom.nl', 'https://www.allesoverseks.be', 'https://www.telegraaf.nl', 'https://sense.info']</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>['https://www.wur.nl', 'https://www.rijksoverheid.nl', 'https://www.klimaat.be', 'https://ec.europa.eu', 'https://www.hier.nu', 'https://www.knaw.nl', 'https://www.ce.nl', 'https://www.climategate.nl', 'https://www.urgenda.nl', 'https://milieudefensie.nl']</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nu.nl', 'https://www.lc.nl', 'https://nos.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nrc.nl', 'https://www.omroepbrabant.nl']</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.volkskrant.nl', 'https://www.volkskrant.nl', 'https://www.nrc.nl', 'https://www.scientias.nl', 'https://www.umcutrecht.nl']</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.volkskrant.nl', 'https://europadecentraal.nl', 'https://www.amnesty.nl', 'https://jalta.nl', 'https://decorrespondent.nl', 'https://www.socialevraagstukken.nl', 'https://www.rijksoverheid.nl', 'https://www.europa-nu.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://www.thuisarts.nl', 'https://fiom.nl', 'https://www.allesoverseks.be', 'https://www.telegraaf.nl', 'https://sense.info']</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://www.urgenda.nl', 'https://www.climategate.nl', 'https://www.climategate.nl', 'https://milieudefensie.nl']</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nu.nl', 'https://www.lc.nl', 'https://nos.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nrc.nl', 'https://www.omroepbrabant.nl']</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.umcutrecht.nl', 'https://www.thuisvaccinatie.nl', 'https://www.volkskrant.nl', 'https://www.nrc.nl', 'https://www.scientias.nl', 'https://dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.volkskrant.nl', 'https://www.politie.nl', 'https://europadecentraal.nl', 'https://www.amnesty.nl', 'https://jalta.nl', 'https://decorrespondent.nl', 'https://www.rijksoverheid.nl', 'https://www.europa-nu.nl', 'https://www.socialevraagstukken.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://www.thuisarts.nl', 'https://fiom.nl', 'https://www.allesoverseks.be', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl']</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>['https://www.wur.nl', 'https://www.rijksoverheid.nl', 'https://www.klimaat.be', 'https://ec.europa.eu', 'https://www.hier.nu', 'https://www.ce.nl', 'https://www.knaw.nl', 'https://www.climategate.nl', 'https://www.urgenda.nl', 'https://www.lne.be']</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nu.nl', 'https://www.lc.nl', 'https://www.nrc.nl', 'https://www.rtlnieuws.nl', 'https://eenvandaag.avrotros.nl', 'https://www.ed.nl', 'houvanarnhem.nl']</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.scientias.nl', 'https://www.nrc.nl', 'https://www.volkskrant.nl', 'https://www.umcutrecht.nl', 'https://mens-en-gezondheid.infonu.nl']</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.volkskrant.nl', 'https://www.politie.nl', 'https://jalta.nl', 'https://decorrespondent.nl', 'https://www.rijksoverheid.nl', 'https://www.socialevraagstukken.nl', 'https://www.europa-nu.nl', 'ind.nl', 'https://europadecentraal.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -540,396 +812,1076 @@
           <t>['https://www.rijksoverheid.nl', 'https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.schreeuwomleven.nl', 'https://www.gezondheidsnet.nl']</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.urgenda.nl', 'https://www.climategate.nl', 'https://milieudefensie.nl', 'https://www.hier.nu', 'https://www.clo.nl']</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.lc.nl', 'https://www.nrc.nl', 'https://eenvandaag.avrotros.nl', 'https://www.omroepbrabant.nl', 'https://www.nu.nl', 'https://www.ed.nl']</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.scientias.nl', 'https://www.nrc.nl', 'https://www.umcutrecht.nl', 'https://www.ggdreisvaccinaties.nl', 'https://dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.volkskrant.nl', 'https://www.rijksoverheid.nl', 'https://jalta.nl', 'https://www.europa-nu.nl', 'https://www.amnesty.nl', 'https://europadecentraal.nl', 'https://decorrespondent.nl', 'https://www.socialevraagstukken.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.schreeuwomleven.nl', 'https://www.gezondheidsnet.nl']</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.urgenda.nl', 'https://milieudefensie.nl', 'https://www.climategate.nl', 'https://www.hier.nu', 'https://www.clo.nl']</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.lc.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nrc.nl', 'https://www.nu.nl', 'https://www.omroepbrabant.nl', 'https://www.destentor.nl', 'https://joop.bnnvara.nl']</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.scientias.nl', 'https://www.nrc.nl', 'https://www.umcutrecht.nl', 'https://dekennisvannu.nl', 'https://www.ggdreisvaccinaties.nl']</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.volkskrant.nl', 'https://www.rijksoverheid.nl', 'https://jalta.nl', 'https://www.europa-nu.nl', 'https://www.amnesty.nl', 'https://europadecentraal.nl', 'https://www.socialevraagstukken.nl', 'https://decorrespondent.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.schreeuwomleven.nl', 'https://www.telegraaf.nl', 'https://www.gezondheidsnet.nl']</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.climategate.nl', 'https://www.climategate.nl', 'https://www.urgenda.nl', 'https://milieudefensie.nl', 'https://www.hier.nu']</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://nl.wikipedia.org', 'https://www.nrc.nl', 'houvanarnhem.nl', 'https://eenvandaag.avrotros.nl', 'https://eenvandaag.avrotros.nl', 'https://nos.nl', 'https://www.ed.nl']</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.scientias.nl', 'https://www.nrc.nl', 'https://www.umcutrecht.nl', 'https://dekennisvannu.nl', 'https://www.volkskrant.nl']</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.rijksoverheid.nl', 'https://www.volkskrant.nl', 'https://europadecentraal.nl', 'https://decorrespondent.nl', 'https://jalta.nl', 'https://www.amnesty.nl', 'https://www.europa-nu.nl', 'https://www.socialevraagstukken.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl', 'https://www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.urgenda.nl', 'https://www.klimaat.be', 'https://www.climategate.nl', 'https://www.climategate.nl', 'https://www.hier.nu', 'https://milieudefensie.nl']</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://nl.wikipedia.org', 'https://www.nrc.nl', 'houvanarnhem.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nu.nl', 'https://joop.bnnvara.nl', 'https://nos.nl']</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.rtlnieuws.nl', 'https://www.scientias.nl', 'https://www.umcutrecht.nl', 'https://www.nrc.nl', 'https://www.ggdreisvaccinaties.nl']</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://europadecentraal.nl', 'https://www.europa-nu.nl', 'https://www.volkskrant.nl', 'https://www.volkskrant.nl', 'https://www.parool.nl', 'https://www.rijksoverheid.nl', 'https://www.rijksoverheid.nl', 'https://www.socialevraagstukken.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.gezondheidsplein.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl', 'https://www.allesoverseks.be']</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.ce.nl', 'https://www.hier.nu', 'https://www.knaw.nl', 'https://www.climategate.nl', 'https://www.urgenda.nl', 'https://www.lne.be']</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://nl.wikipedia.org', 'https://www.nrc.nl', 'https://joop.bnnvara.nl', 'https://www.ed.nl', 'https://eenvandaag.avrotros.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nu.nl']</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.scientias.nl', 'https://www.volkskrant.nl', 'https://mens-en-gezondheid.infonu.nl', 'https://www.nrc.nl', 'https://www.umcutrecht.nl']</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.rijksoverheid.nl', 'https://europadecentraal.nl', 'https://www.volkskrant.nl', 'https://www.amnesty.nl', 'https://decorrespondent.nl', 'https://jalta.nl', 'https://www.socialevraagstukken.nl', 'https://www.europa-nu.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl', 'https://www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.urgenda.nl', 'https://www.klimaat.be', 'https://www.climategate.nl', 'https://www.climategate.nl', 'https://milieudefensie.nl', 'https://www.hier.nu']</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nrc.nl', 'https://nl.wikipedia.org', 'houvanarnhem.nl', 'https://eenvandaag.avrotros.nl', 'https://eenvandaag.avrotros.nl', 'https://joop.bnnvara.nl', 'https://www.nu.nl']</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.scientias.nl', 'https://www.umcutrecht.nl', 'https://www.nrc.nl', 'https://dekennisvannu.nl', 'https://www.volkskrant.nl']</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.rijksoverheid.nl', 'https://www.volkskrant.nl', 'https://europadecentraal.nl', 'https://decorrespondent.nl', 'https://www.amnesty.nl', 'https://www.europa-nu.nl', 'https://jalta.nl', 'https://www.socialevraagstukken.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl', 'https://www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.urgenda.nl', 'https://www.klimaat.be', 'https://www.climategate.nl', 'https://www.climategate.nl', 'https://milieudefensie.nl', 'https://www.hier.nu']</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nrc.nl', 'https://nl.wikipedia.org', 'houvanarnhem.nl', 'https://eenvandaag.avrotros.nl', 'https://joop.bnnvara.nl', 'https://nos.nl', 'https://www.nu.nl']</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.scientias.nl', 'https://www.umcutrecht.nl', 'https://www.nrc.nl', 'https://www.ggdreisvaccinaties.nl', 'https://www.volkskrant.nl']</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.rijksoverheid.nl', 'https://www.volkskrant.nl', 'https://europadecentraal.nl', 'https://decorrespondent.nl', 'https://www.amnesty.nl', 'https://www.europa-nu.nl', 'https://jalta.nl', 'https://www.socialevraagstukken.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl', 'https://www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.urgenda.nl', 'https://www.klimaat.be', 'https://www.climategate.nl', 'https://www.climategate.nl', 'https://www.hier.nu', 'https://milieudefensie.nl']</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://nl.wikipedia.org', 'https://www.nrc.nl', 'houvanarnhem.nl', 'https://eenvandaag.avrotros.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nu.nl', 'https://nos.nl']</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.rtlnieuws.nl', 'https://www.scientias.nl', 'https://www.umcutrecht.nl', 'https://www.nrc.nl', 'https://www.ggdreisvaccinaties.nl']</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.rijksoverheid.nl', 'https://www.volkskrant.nl', 'https://europadecentraal.nl', 'https://www.amnesty.nl', 'https://decorrespondent.nl', 'https://www.europa-nu.nl', 'https://jalta.nl', 'https://www.socialevraagstukken.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl', 'https://www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.urgenda.nl', 'https://www.klimaat.be', 'https://milieudefensie.nl', 'https://www.climategate.nl', 'https://www.hier.nu', 'https://www.clo.nl']</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://nl.wikipedia.org', 'https://www.nrc.nl', 'https://eenvandaag.avrotros.nl', 'houvanarnhem.nl', 'https://nos.nl', 'https://nos.nl', 'https://www.nu.nl']</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.rtlnieuws.nl', 'https://www.scientias.nl', 'https://www.umcutrecht.nl', 'https://www.ggdreisvaccinaties.nl', 'https://www.volkskrant.nl']</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.rijksoverheid.nl', 'https://www.volkskrant.nl', 'https://europadecentraal.nl', 'https://www.amnesty.nl', 'https://decorrespondent.nl', 'https://www.europa-nu.nl', 'https://www.socialevraagstukken.nl', 'https://www.nd.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl/www.rijksoverheid.nl', 'https://www.bloemenhove.nl/www.bloemenhove.nl', 'https://www.bloemenhove.nl/www.bloemenhove.nl', 'https://www.thuisarts.nl/www.thuisarts.nl', 'https://www.trouw.nl/www.trouw.nl', 'https://www.gezondheidsplein.nl/www.gezondheidsplein.nl', 'https://fiom.nl/fiom.nl', 'https://www.schreeuwomleven.nl/www.schreeuwomleven.nl', 'https://www.telegraaf.nl/www.telegraaf.nl', 'https://www.telegraaf.nl/www.telegraaf.nl']</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl/www.rijksoverheid.nl', 'https://www.wur.nl/www.wur.nl', 'PDFhttps://www.ce.nl/www.ce.nl', 'https://www.urgenda.nl/www.urgenda.nl', 'https://ec.europa.eu/ec.europa.eu', 'https://www.klimaat.be/www.klimaat.be', 'https://www.hier.nu/www.hier.nu', 'https://milieudefensie.nl/milieudefensie.nl', 'https://www.climategate.nl/www.climategate.nl', 'https://www.clo.nl/www.clo.nl']</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl/www.ad.nl', 'https://www.ad.nl/www.ad.nl', 'https://www.volkskrant.nl/www.volkskrant.nl', 'https://www.trouw.nl/www.trouw.nl', 'https://www.nrc.nl/www.nrc.nl', 'https://eenvandaag.avrotros.nl/eenvandaag.avrotros.nl', 'https://eenvandaag.avrotros.nl/eenvandaag.avrotros.nl', 'https://nl.wikipedia.org/nl.wikipedia.org', 'http://houvanarnhem.nl/houvanarnhem.nl', 'https://www.nu.nl/www.nu.nl']</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl/rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl/www.nvkp.nl', 'PDFhttps://www.wanttoknow.nl/www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl/stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl/www.thuisvaccinatie.nl', 'https://www.scientias.nl/www.scientias.nl', 'https://www.volkskrant.nl/www.volkskrant.nl', 'https://www.umcutrecht.nl/www.umcutrecht.nl', 'https://mens-en-gezondheid.infonu.nl/mens-en-gezondheid.infonu.nl', 'https://dekennisvannu.nl/dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org/nl.wikipedia.org', 'https://www.politie.nl/www.politie.nl', 'https://www.rijksoverheid.nl/www.rijksoverheid.nl', 'https://www.volkskrant.nl/www.volkskrant.nl', 'https://europadecentraal.nl/europadecentraal.nl', 'https://www.amnesty.nl/www.amnesty.nl', 'https://decorrespondent.nl/decorrespondent.nl', 'https://www.nd.nl/www.nd.nl', 'https://www.europa-nu.nl/www.europa-nu.nl', 'https://jalta.nl/jalta.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://fiom.nl', 'https://www.schreeuwomleven.nl', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl']</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://www.urgenda.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://milieudefensie.nl', 'https://www.climategate.nl', 'https://www.clo.nl']</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nrc.nl', 'https://eenvandaag.avrotros.nl', 'https://eenvandaag.avrotros.nl', 'https://nl.wikipedia.org', 'houvanarnhem.nl', 'https://www.nu.nl']</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.scientias.nl', 'https://www.umcutrecht.nl', 'https://www.volkskrant.nl', 'https://www.ggdreisvaccinaties.nl', 'https://mens-en-gezondheid.infonu.nl']</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.politie.nl', 'https://www.rijksoverheid.nl', 'https://www.volkskrant.nl', 'https://europadecentraal.nl', 'https://www.amnesty.nl', 'https://decorrespondent.nl', 'https://jalta.nl', 'https://www.nd.nl', 'https://www.europa-nu.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.gezondheidsplein.nl', 'https://www.trouw.nl', 'https://fiom.nl', 'https://www.schreeuwomleven.nl', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl']</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://www.urgenda.nl', 'https://ec.europa.eu', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://milieudefensie.nl', 'https://www.clo.nl', 'https://www.climategate.nl']</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nrc.nl', 'https://eenvandaag.avrotros.nl', 'https://eenvandaag.avrotros.nl', 'https://nl.wikipedia.org', 'houvanarnhem.nl']</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.nvkp.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.rtlnieuws.nl', 'https://www.umcutrecht.nl', 'https://www.scientias.nl', 'https://www.ggdreisvaccinaties.nl', 'https://www.volkskrant.nl']</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.rijksoverheid.nl', 'https://www.politie.nl', 'https://www.amnesty.nl', 'https://europadecentraal.nl', 'https://decorrespondent.nl', 'https://www.volkskrant.nl', 'https://www.parool.nl', 'https://www.europa-nu.nl', 'https://jalta.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.gezondheidsplein.nl', 'https://www.trouw.nl', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl', 'https://fiom.nl', 'https://www.gezondheidsnet.nl']</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://www.urgenda.nl', 'https://ec.europa.eu', 'https://milieudefensie.nl', 'https://www.clo.nl', 'https://www.klimaat.be', 'https://www.hier.nu', 'https://www.climategate.nl']</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.ad.nl', 'https://www.volkskrant.nl', 'https://nl.wikipedia.org', 'https://www.trouw.nl', 'https://www.nrc.nl', 'https://eenvandaag.avrotros.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nu.nl']</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://rijksvaccinatieprogramma.nl', 'https://www.wanttoknow.nl', 'https://www.nvkp.nl', 'https://www.thuisvaccinatie.nl', 'https://www.rtlnieuws.nl', 'https://www.scientias.nl', 'https://www.umcutrecht.nl', 'https://www.nrc.nl', 'https://www.larsvanhemmen.nl']</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.rijksoverheid.nl', 'https://www.politie.nl', 'https://www.amnesty.nl', 'https://europadecentraal.nl', 'https://www.volkskrant.nl', 'https://www.volkskrant.nl', 'https://decorrespondent.nl', 'https://decorrespondent.nl', 'https://www.dagelijksestandaard.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>['www.rijksoverheid.nl', 'www.bloemenhove.nl', 'www.bloemenhove.nl', 'www.thuisarts.nl', 'www.gezondheidsplein.nl', 'www.trouw.nl', 'fiom.nl', 'www.telegraaf.nl', 'www.schreeuwomleven.nl', 'www.gezondheidsnet.nl']</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>['www.rijksoverheid.nl', 'www.wur.nl', 'www.ce.nl', 'ec.europa.eu', 'www.urgenda.nl', 'www.clo.nl', 'milieudefensie.nl', 'www.klimaat.be', 'www.hier.nu', 'www.knaw.nl']</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>['www.ad.nl', 'www.ad.nl', 'www.volkskrant.nl', 'nl.wikipedia.org', 'www.trouw.nl', 'www.nrc.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'www.nu.nl']</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>['rijksvaccinatieprogramma.nl', 'www.wanttoknow.nl', 'www.nvkp.nl', 'stichtingvaccinvrij.nl', 'www.thuisvaccinatie.nl', 'www.scientias.nl', 'www.rtlnieuws.nl', 'www.umcutrecht.nl', 'www.nieuwetijds-kindercoach.nl', 'dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>['nl.wikipedia.org', 'www.rijksoverheid.nl', 'www.politie.nl', 'www.amnesty.nl', 'europadecentraal.nl', 'www.volkskrant.nl', 'www.volkskrant.nl', 'decorrespondent.nl', 'decorrespondent.nl', 'jalta.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl/www.rijksoverheid.nl', 'https://www.bloemenhove.nl/www.bloemenhove.nl', 'https://www.bloemenhove.nl/www.bloemenhove.nl', 'https://www.thuisarts.nl/www.thuisarts.nl', 'https://www.gezondheidsplein.nl/www.gezondheidsplein.nl', 'https://www.trouw.nl/www.trouw.nl', 'https://fiom.nl/fiom.nl', 'https://www.telegraaf.nl/www.telegraaf.nl', 'https://www.schreeuwomleven.nl/www.schreeuwomleven.nl', 'https://www.gezondheidsnet.nl/www.gezondheidsnet.nl']</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl/www.rijksoverheid.nl', 'https://www.wur.nl/www.wur.nl', 'https://www.ce.nl/www.ce.nl', 'https://ec.europa.eu/ec.europa.eu', 'https://www.urgenda.nl/www.urgenda.nl', 'https://www.clo.nl/www.clo.nl', 'https://milieudefensie.nl/milieudefensie.nl', 'https://www.klimaat.be/www.klimaat.be', 'https://www.hier.nu/www.hier.nu', 'https://www.climategate.nl/www.climategate.nl']</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl/www.ad.nl', 'https://www.ad.nl/www.ad.nl', 'https://www.volkskrant.nl/www.volkskrant.nl', 'https://nl.wikipedia.org/nl.wikipedia.org', 'https://www.trouw.nl/www.trouw.nl', 'https://www.nrc.nl/www.nrc.nl', 'https://eenvandaag.avrotros.nl/eenvandaag.avrotros.nl', 'https://eenvandaag.avrotros.nl/eenvandaag.avrotros.nl', 'https://www.nu.nl/www.nu.nl']</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl/rijksvaccinatieprogramma.nl', 'https://www.wanttoknow.nl/www.wanttoknow.nl', 'https://www.nvkp.nl/www.nvkp.nl', 'https://stichtingvaccinvrij.nl/stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl/www.thuisvaccinatie.nl', 'https://www.scientias.nl/www.scientias.nl', 'https://www.rtlnieuws.nl/www.rtlnieuws.nl', 'https://www.umcutrecht.nl/www.umcutrecht.nl', 'https://www.nieuwetijds-kindercoach.nl/www.nieuwetijds-kindercoach.nl', 'https://dekennisvannu.nl/dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org/nl.wikipedia.org', 'https://www.rijksoverheid.nl/www.rijksoverheid.nl', 'https://www.politie.nl/www.politie.nl', 'https://www.amnesty.nl/www.amnesty.nl', 'https://europadecentraal.nl/europadecentraal.nl', 'https://www.volkskrant.nl/www.volkskrant.nl', 'https://decorrespondent.nl/decorrespondent.nl', 'https://decorrespondent.nl/decorrespondent.nl', 'https://jalta.nl/jalta.nl', 'https://www.ad.nl/www.ad.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="B31" t="inlineStr"/>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.gezondheidsplein.nl', 'https://www.trouw.nl', 'https://www.telegraaf.nl', 'https://fiom.nl', 'https://www.schreeuwomleven.nl', 'https://www.gezondheidsnet.nl']</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.ce.nl', 'https://ec.europa.eu', 'https://www.urgenda.nl', 'https://www.clo.nl', 'https://www.klimaat.be', 'https://milieudefensie.nl', 'https://www.hier.nu', 'https://www.knaw.nl']</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.ad.nl', 'https://www.volkskrant.nl', 'https://nl.wikipedia.org', 'https://www.trouw.nl', 'https://www.nrc.nl', 'https://eenvandaag.avrotros.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nu.nl']</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.wanttoknow.nl', 'https://www.nvkp.nl', 'https://stichtingvaccinvrij.nl', 'https://www.scientias.nl', 'https://www.thuisvaccinatie.nl', 'https://www.rtlnieuws.nl', 'https://dekennisvannu.nl', 'https://www.umcutrecht.nl', 'https://www.nieuwetijds-kindercoach.nl']</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.rijksoverheid.nl', 'https://www.politie.nl', 'https://www.amnesty.nl', 'https://europadecentraal.nl', 'https://www.volkskrant.nl', 'https://decorrespondent.nl', 'https://decorrespondent.nl', 'https://jalta.nl', 'https://www.dagelijksestandaard.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="B32" t="inlineStr"/>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl/www.rijksoverheid.nl', 'https://www.bloemenhove.nl/www.bloemenhove.nl', 'https://www.bloemenhove.nl/www.bloemenhove.nl', 'https://www.thuisarts.nl/www.thuisarts.nl', 'https://www.gezondheidsplein.nl/www.gezondheidsplein.nl', 'https://www.trouw.nl/www.trouw.nl', 'https://www.telegraaf.nl/www.telegraaf.nl', 'https://fiom.nl/fiom.nl', 'https://www.schreeuwomleven.nl/www.schreeuwomleven.nl', 'https://www.gezondheidsnet.nl/www.gezondheidsnet.nl']</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl/www.rijksoverheid.nl', 'https://www.wur.nl/www.wur.nl', 'https://www.ce.nl/www.ce.nl', 'https://ec.europa.eu/ec.europa.eu', 'https://www.urgenda.nl/www.urgenda.nl', 'https://www.clo.nl/www.clo.nl', 'https://www.klimaat.be/www.klimaat.be', 'https://milieudefensie.nl/milieudefensie.nl', 'https://www.hier.nu/www.hier.nu', 'https://www.knaw.nl/www.knaw.nl']</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl/www.ad.nl', 'https://www.ad.nl/www.ad.nl', 'https://www.volkskrant.nl/www.volkskrant.nl', 'https://nl.wikipedia.org/nl.wikipedia.org', 'https://www.trouw.nl/www.trouw.nl', 'https://www.nrc.nl/www.nrc.nl', 'https://eenvandaag.avrotros.nl/eenvandaag.avrotros.nl', 'https://eenvandaag.avrotros.nl/eenvandaag.avrotros.nl', 'https://www.nu.nl/www.nu.nl']</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl/rijksvaccinatieprogramma.nl', 'https://www.wanttoknow.nl/www.wanttoknow.nl', 'https://www.nvkp.nl/www.nvkp.nl', 'https://stichtingvaccinvrij.nl/stichtingvaccinvrij.nl', 'https://www.scientias.nl/www.scientias.nl', 'https://www.thuisvaccinatie.nl/www.thuisvaccinatie.nl', 'https://www.rtlnieuws.nl/www.rtlnieuws.nl', 'https://www.umcutrecht.nl/www.umcutrecht.nl', 'https://www.nieuwetijds-kindercoach.nl/www.nieuwetijds-kindercoach.nl', 'https://dekennisvannu.nl/dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org/nl.wikipedia.org', 'https://www.rijksoverheid.nl/www.rijksoverheid.nl', 'https://www.politie.nl/www.politie.nl', 'https://www.amnesty.nl/www.amnesty.nl', 'https://europadecentraal.nl/europadecentraal.nl', 'https://www.volkskrant.nl/www.volkskrant.nl', 'https://decorrespondent.nl/decorrespondent.nl', 'https://decorrespondent.nl/decorrespondent.nl', 'https://www.dagelijksestandaard.nl/www.dagelijksestandaard.nl', 'https://jalta.nl/jalta.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="B33" t="inlineStr"/>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>['www.bloemenhove.nl', 'www.bloemenhove.nl', 'www.gezondheidsplein.nl', 'www.thuisarts.nl', 'www.trouw.nl', 'www.telegraaf.nl', 'fiom.nl', 'www.ad.nl', 'www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>['www.rijksoverheid.nl', 'www.wur.nl', 'ec.europa.eu', 'www.klimaat.be', 'www.urgenda.nl', 'www.knaw.nl', 'www.hier.nu', 'www.clo.nl', 'www.lne.be']</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>['www.ad.nl', 'www.ad.nl', 'www.volkskrant.nl', 'www.trouw.nl', 'www.nrc.nl', 'www.nu.nl', 'www.rtlnieuws.nl', 'eenvandaag.avrotros.nl', 'nos.nl']</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>['rijksvaccinatieprogramma.nl', 'www.wanttoknow.nl', 'WantToKnow.nlPDF', 'stichtingvaccinvrij.nl', 'www.thuisvaccinatie.nl', 'www.scientias.nl', 'www.rtlnieuws.nl', 'mens-en-gezondheid.infonu.nl', 'www.larsvanhemmen.nl', 'www.volkskrant.nl']</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>['www.rijksoverheid.nl', 'www.politie.nl', 'www.amnesty.nl', 'europadecentraal.nl', 'decorrespondent.nl', 'decorrespondent.nl', 'eur-lex.europa.eu', 'eur-lex.europa.eu', 'www.volkskrant.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>['www.bloemenhove.nl', 'www.bloemenhove.nl', 'www.thuisarts.nl', 'www.trouw.nl', 'www.gezondheidsplein.nl', 'www.telegraaf.nl', 'fiom.nl', 'www.schreeuwomleven.nl', 'www.gezondheidsnet.nl']</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>['www.rijksoverheid.nl', 'www.wur.nl', 'www.urgenda.nl', 'ec.europa.eu', 'www.clo.nl', 'www.klimaat.be', 'milieudefensie.nl', 'www.knaw.nl', 'www.hier.nu']</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>['www.ad.nl', 'www.ad.nl', 'www.volkskrant.nl', 'www.trouw.nl', 'www.nrc.nl', 'www.nu.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'joop.bnnvara.nl']</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>['rijksvaccinatieprogramma.nl', 'www.wanttoknow.nl', 'www.nvkp.nl', 'stichtingvaccinvrij.nl', 'www.thuisvaccinatie.nl', 'www.scientias.nl', 'www.rtlnieuws.nl', 'www.larsvanhemmen.nl', 'www.ggdreisvaccinaties.nl', 'www.umcutrecht.nl']</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>['www.rijksoverheid.nl', 'www.politie.nl', 'www.amnesty.nl', 'europadecentraal.nl', 'decorrespondent.nl', 'decorrespondent.nl', 'www.volkskrant.nl', 'www.volkskrant.nl', 'eur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="B35" t="inlineStr"/>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>['https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://www.telegraaf.nl', 'https://fiom.nl', 'https://www.schreeuwomleven.nl', 'https://www.gezondheidsnet.nl']</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://www.urgenda.nl', 'https://ec.europa.eu', 'https://www.clo.nl', 'https://milieudefensie.nl', 'https://www.klimaat.be', 'https://www.knaw.nl', 'https://www.hier.nu']</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>['https://www.ad.nl', 'https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://www.nrc.nl', 'https://www.nu.nl', 'https://eenvandaag.avrotros.nl', 'https://eenvandaag.avrotros.nl', 'https://joop.bnnvara.nl']</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.wanttoknow.nl', 'https://www.nvkp.nl', 'https://stichtingvaccinvrij.nl', 'https://www.thuisvaccinatie.nl', 'https://www.scientias.nl', 'https://www.rtlnieuws.nl', 'https://www.larsvanhemmen.nl', 'https://www.umcutrecht.nl', 'https://www.nrc.nl']</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.politie.nl', 'https://www.amnesty.nl', 'https://europadecentraal.nl', 'https://www.volkskrant.nl', 'https://www.volkskrant.nl', 'https://decorrespondent.nl', 'https://decorrespondent.nl', 'https://eur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="B36" t="inlineStr"/>
-      <c r="C36" t="inlineStr"/>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>['www.bloemenhove.nl', 'www.bloemenhove.nl', 'www.thuisarts.nl', 'www.trouw.nl', 'www.gezondheidsplein.nl', 'fiom.nl', 'www.telegraaf.nl', 'www.telegraaf.nl', 'www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>['www.rijksoverheid.nl', 'www.wur.nl', 'www.clo.nl', 'www.urgenda.nl', 'ec.europa.eu', 'www.klimaat.be', 'milieudefensie.nl', 'www.knaw.nl', 'www.hier.nu']</t>
+        </is>
+      </c>
       <c r="D36" t="inlineStr">
         <is>
           <t>['www.ad.nl', 'www.ad.nl', 'www.volkskrant.nl', 'www.trouw.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'www.nrc.nl', 'www.nu.nl']</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>['rijksvaccinatieprogramma.nl', 'www.wanttoknow.nl', 'www.nvkp.nl', 'stichtingvaccinvrij.nl', 'www.thuisvaccinatie.nl', 'www.scientias.nl', 'www.umcutrecht.nl', 'www.nieuwetijds-kindercoach.nl', 'www.ggdreisvaccinaties.nl', 'dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>['nl.wikipedia.org', 'www.rijksoverheid.nl', 'www.politie.nl', 'www.amnesty.nl', 'www.volkskrant.nl', 'www.volkskrant.nl', 'europadecentraal.nl', 'decorrespondent.nl', 'eur-lex.europa.eu', 'eur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B37" t="inlineStr"/>
-      <c r="C37" t="inlineStr"/>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>['www.bloemenhove.nl', 'www.bloemenhove.nl', 'www.thuisarts.nl', 'www.trouw.nl', 'www.gezondheidsplein.nl', 'fiom.nl', 'www.telegraaf.nl', 'www.telegraaf.nl', 'www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>['www.rijksoverheid.nl', 'www.wur.nl', 'www.clo.nl', 'www.urgenda.nl', 'ec.europa.eu', 'www.klimaat.be', 'milieudefensie.nl', 'www.knaw.nl', 'www.climategate.nl']</t>
+        </is>
+      </c>
       <c r="D37" t="inlineStr">
         <is>
           <t>['www.ad.nl', 'www.ad.nl', 'www.volkskrant.nl', 'www.trouw.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'www.nrc.nl', 'www.nu.nl']</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>['rijksvaccinatieprogramma.nl', 'www.wanttoknow.nl', 'stichtingvaccinvrij.nl', 'www.nvkp.nl', 'www.thuisvaccinatie.nl', 'www.scientias.nl', 'www.umcutrecht.nl', 'www.nieuwetijds-kindercoach.nl', 'www.ggdreisvaccinaties.nl', 'dekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>['nl.wikipedia.org', 'www.rijksoverheid.nl', 'www.politie.nl', 'www.amnesty.nl', 'www.volkskrant.nl', 'www.volkskrant.nl', 'europadecentraal.nl', 'decorrespondent.nl', 'eur-lex.europa.eu', 'eur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>['www.bloemenhove.nl', 'www.bloemenhove.nl', 'www.gezondheidsplein.nl', 'www.thuisarts.nl', 'www.trouw.nl', 'www.telegraaf.nl', 'www.telegraaf.nl', 'fiom.nl', 'sense.info']</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>['www.wur.nl', 'www.hier.nu', 'ec.europa.eu', 'www.rijksoverheid.nl', 'www.klimaat.be', 'www.climategate.nl', 'www.climategate.nl', 'www.energievergelijk.nl', 'www.urgenda.nl']</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>['www.ad.nl', 'www.ad.nl', 'www.volkskrant.nl', 'www.trouw.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'www.nu.nl', 'joop.bnnvara.nl', 'www.nrc.nl']</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>['www.wanttoknow.nl', 'www.nvkp.nl', 'stichtingvaccinvrij.nl', 'www.thuisvaccinatie.nl', 'www.scientias.nl', 'www.volkskrant.nl', 'mens-en-gezondheid.infonu.nl', 'www.umcutrecht.nl', 'www.laatjevaccineren.be']</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>['www.rijksoverheid.nl', 'www.politie.nl', 'www.amnesty.nl', 'europadecentraal.nl', 'eur-lex.europa.eu', 'eur-lex.europa.eu', 'decorrespondent.nl', 'www.volkskrant.nl', 'www.volkskrant.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr"/>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>['www.bloemenhove.nl', 'www.bloemenhove.nl', 'www.thuisarts.nl', 'www.trouw.nl', 'www.gezondheidsplein.nl', 'www.telegraaf.nl', 'www.telegraaf.nl', 'fiom.nl', 'www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>['www.rijksoverheid.nl', 'www.wur.nl', 'ec.europa.eu', 'www.knaw.nl', 'www.clo.nl', 'www.urgenda.nl', 'milieudefensie.nl', 'nl.wikipedia.org', 'michielhaas.nl']</t>
+        </is>
+      </c>
       <c r="D39" t="inlineStr">
         <is>
           <t>['www.ad.nl', 'www.volkskrant.nl', 'www.trouw.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'www.nu.nl', 'www.nrc.nl', 'nos.nl']</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>['rijksvaccinatieprogramma.nl', 'www.wanttoknow.nl', 'stichtingvaccinvrij.nl', 'www.nvkp.nl', 'www.thuisvaccinatie.nl', 'www.scientias.nl', 'www.umcutrecht.nl', 'dekennisvannu.nl', 'mens-en-gezondheid.infonu.nl', 'www.nieuwetijds-kindercoach.nl']</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>['nl.wikipedia.org', 'www.rijksoverheid.nl', 'www.politie.nl', 'decorrespondent.nl', 'www.volkskrant.nl', 'www.volkskrant.nl', 'europadecentraal.nl', 'jalta.nl', 'eur-lex.europa.eu', 'www2.openvld.be']</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="B40" t="inlineStr"/>
-      <c r="C40" t="inlineStr"/>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>['https://www.bloemenhove.nl', 'https://www.bloemenhove.nl', 'https://www.thuisarts.nl', 'https://www.trouw.nl', 'https://www.gezondheidsplein.nl', 'https://www.telegraaf.nl', 'https://www.telegraaf.nl', 'https://fiom.nl', 'https://www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>['https://www.rijksoverheid.nl', 'https://www.wur.nl', 'https://ec.europa.eu', 'https://www.knaw.nl', 'https://www.clo.nl', 'https://www.urgenda.nl', 'https://milieudefensie.nl', 'https://nl.wikipedia.org', 'https://michielhaas.nl']</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr">
         <is>
           <t>['https://www.ad.nl', 'https://www.volkskrant.nl', 'https://www.trouw.nl', 'https://eenvandaag.avrotros.nl', 'https://www.nu.nl', 'https://www.nrc.nl', 'https://nos.nl', 'https://joop.bnnvara.nl']</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>['https://rijksvaccinatieprogramma.nl', 'https://www.wanttoknow.nl', 'https://stichtingvaccinvrij.nl', 'https://www.nvkp.nl', 'https://www.thuisvaccinatie.nl', 'https://www.scientias.nl', 'https://dekennisvannu.nl', 'https://www.umcutrecht.nl', 'https://www.nieuwetijds-kindercoach.nl', 'https://www.volkskrant.nl']</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>['https://nl.wikipedia.org', 'https://www.rijksoverheid.nl', 'https://www.politie.nl', 'https://decorrespondent.nl', 'https://www.volkskrant.nl', 'https://www.volkskrant.nl', 'https://europadecentraal.nl', 'https://jalta.nl', 'https://eur-lex.europa.eu', 'https://www2.openvld.be']</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="B41" t="inlineStr"/>
-      <c r="C41" t="inlineStr"/>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>['www.bloemenhove.nl', 'www.bloemenhove.nl', 'www.thuisarts.nl', 'www.trouw.nl', 'www.gezondheidsplein.nl', 'fiom.nl', 'www.telegraaf.nl', 'www.telegraaf.nl', 'www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>['www.rijksoverheid.nl', 'www.wur.nl', 'www.klimaat.be', 'ec.europa.eu', 'www.urgenda.nl', 'milieudefensie.nl', 'www.knaw.nl', 'www.hier.nu', 'www.clo.nl']</t>
+        </is>
+      </c>
       <c r="D41" t="inlineStr">
         <is>
           <t>['www.ad.nl', 'www.volkskrant.nl', 'www.trouw.nl', 'www.nu.nl', 'eenvandaag.avrotros.nl', 'nos.nl', 'www.nrc.nl', 'www.rtvoost.nl']</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>['rijksvaccinatieprogramma.nl', 'www.wanttoknow.nl', 'stichtingvaccinvrij.nl', 'www.nvkp.nl', 'www.thuisvaccinatie.nl', 'www.scientias.nl', 'www.umcutrecht.nl', 'www.nieuwetijds-kindercoach.nl', 'www.ggdreisvaccinaties.nl', 'www.volkskrant.nl']</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>['nl.wikipedia.org', 'www.rijksoverheid.nl', 'www.politie.nl', 'decorrespondent.nl', 'www.amnesty.nl', 'www.volkskrant.nl', 'www.volkskrant.nl', 'europadecentraal.nl', 'jalta.nl', 'eur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="B42" t="inlineStr"/>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>['www.bloemenhove.nl', 'www.bloemenhove.nl', 'www.thuisarts.nl', 'www.trouw.nl', 'www.gezondheidsplein.nl', 'fiom.nl', 'www.telegraaf.nl', 'www.telegraaf.nl', 'www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>['www.rijksoverheid.nl', 'www.wur.nl', 'www.klimaat.be', 'ec.europa.eu', 'www.urgenda.nl', 'milieudefensie.nl', 'www.hier.nu', 'www.knaw.nl', 'www.clo.nl']</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>['www.ad.nl', 'www.volkskrant.nl', 'www.trouw.nl', 'www.nu.nl', 'eenvandaag.avrotros.nl', 'www.nrc.nl', 'nos.nl', 'www.rtvoost.nl', 'www.omroepbrabant.nl']</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>['rijksvaccinatieprogramma.nl', 'www.wanttoknow.nl', 'stichtingvaccinvrij.nl', 'www.nvkp.nl', 'www.thuisvaccinatie.nl', 'www.scientias.nl', 'www.umcutrecht.nl', 'www.nieuwetijds-kindercoach.nl', 'www.volkskrant.nl', 'www.rivm.nl']</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>['nl.wikipedia.org', 'www.rijksoverheid.nl', 'www.politie.nl', 'decorrespondent.nl', 'www.amnesty.nl', 'www.volkskrant.nl', 'www.volkskrant.nl', 'europadecentraal.nl', 'jalta.nl', 'eur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="B43" t="inlineStr"/>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>['www.bloemenhove.nl', 'www.bloemenhove.nl', 'www.thuisarts.nl', 'www.trouw.nl', 'www.gezondheidsplein.nl', 'fiom.nl', 'www.telegraaf.nl', 'www.telegraaf.nl', 'www.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>['www.wur.nl', 'www.hier.nu', 'www.rijksoverheid.nl', 'ec.europa.eu', 'www.klimaat.be', 'www.ce.nl', 'www.climategate.nl', 'www.climategate.nl', 'www.energievergelijk.nl', 'www.urgenda.nl']</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>['www.ad.nl', 'www.volkskrant.nl', 'www.trouw.nl', 'www.nu.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'www.nrc.nl', 'nos.nl', 'www.omroepbrabant.nl']</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>['www.wanttoknow.nl', 'www.nvkp.nl', 'stichtingvaccinvrij.nl', 'www.thuisvaccinatie.nl', 'www.scientias.nl', 'mens-en-gezondheid.infonu.nl', 'www.volkskrant.nl', 'www.umcutrecht.nl', 'www.laatjevaccineren.be']</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>['nl.wikipedia.org', 'www.rijksoverheid.nl', 'www.politie.nl', 'www.amnesty.nl', 'decorrespondent.nl', 'europadecentraal.nl', 'www.volkskrant.nl', 'jalta.nl', 'eur-lex.europa.eu', 'www.europarl.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="B44" t="inlineStr"/>
-      <c r="C44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>['behandelingwww.bloemenhove.nl', 'Bloemenhovewww.bloemenhove.nl', 'Thuisartswww.thuisarts.nl', 'Trouwwww.trouw.nl', 'www.gezondheidsplein.nl', 'Fiomfiom.nl', 'www.telegraaf.nl', 'www.telegraaf.nl', 'Levenwww.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>['Rijksoverheidwww.rijksoverheid.nl', 'WURwww.wur.nl', 'Klimaat.bewww.klimaat.be', 'www.clo.nl', 'Commissionec.europa.eu', 'www.urgenda.nl', 'Milieudefensiemilieudefensie.nl', 'HIERwww.hier.nu', 'www.knaw.nl']</t>
+        </is>
+      </c>
       <c r="D44" t="inlineStr">
         <is>
           <t>['AD.nlwww.ad.nl', 'Volkskrantwww.volkskrant.nl', 'www.trouw.nl', 'eenvandaag.avrotros.nl', 'www.nu.nl', 'NRCwww.nrc.nl', 'nos.nl', 'nos.nl']</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr"/>
-      <c r="F44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>['Rijksvaccinatieprogramma.nlrijksvaccinatieprogramma.nl', 'WantToKnowwww.wanttoknow.nl', 'Vaccinvrijstichtingvaccinvrij.nl', 'gevolgen?www.nvkp.nl', 'meer!www.thuisvaccinatie.nl', 'Scientiaswww.scientias.nl', 'Utrechtwww.umcutrecht.nl', 'kindercoachwww.nieuwetijds-kindercoach.nl', 'vaccinerendekennisvannu.nl', 'www.volkskrant.nl']</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>['Wikipedianl.wikipedia.org', 'Rijksoverheid.nlwww.rijksoverheid.nl', 'politie.nlwww.politie.nl', 'uitgeprocedeerdenwww.amnesty.nl', 'decorrespondent.nl', 'decentraaleuropadecentraal.nl', 'www.volkskrant.nl', 'www.volkskrant.nl', 'Jaltajalta.nl', 'www.socialevraagstukken.nl']</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>['behandelingwww.bloemenhove.nl', 'Bloemenhovewww.bloemenhove.nl', 'Thuisartswww.thuisarts.nl', 'Trouwwww.trouw.nl', 'www.gezondheidsplein.nl', 'Fiomfiom.nl', 'www.telegraaf.nl', 'www.telegraaf.nl', 'Levenwww.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>['Rijksoverheidwww.rijksoverheid.nl', 'WURwww.wur.nl', 'www.clo.nl', 'Klimaat.bewww.klimaat.be', 'Commissionec.europa.eu', 'www.urgenda.nl', 'Milieudefensiemilieudefensie.nl', 'www.knaw.nl', 'HIERwww.hier.nu']</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>['Adwww.ad.nl', 'Volkskrantwww.volkskrant.nl', 'www.trouw.nl', 'eenvandaag.avrotros.nl', 'nos.nl', 'www.nu.nl', 'NRCwww.nrc.nl', 'joop.bnnvara.nl', 'www.omroepbrabant.nl']</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>['Rijksvaccinatieprogramma.nlrijksvaccinatieprogramma.nl', 'WantToKnowwww.wanttoknow.nl', 'Vaccinvrijstichtingvaccinvrij.nl', 'gevolgen?www.nvkp.nl', 'meer!www.thuisvaccinatie.nl', 'Scientiaswww.scientias.nl', 'Utrechtwww.umcutrecht.nl', 'kindercoachwww.nieuwetijds-kindercoach.nl', 'GGDREISVACCINATIESwww.ggdreisvaccinaties.nl', 'RIVMwww.rivm.nl']</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>['Wikipedianl.wikipedia.org', 'Rijksoverheid.nlwww.rijksoverheid.nl', 'politie.nlwww.politie.nl', 'www.volkskrant.nl', 'decorrespondent.nl', 'decentraaleuropadecentraal.nl', 'uitgeprocedeerdenwww.amnesty.nl', 'Nuwww.europa-nu.nl', 'Jaltajalta.nl', 'EUR-Lexeur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
-      <c r="F46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>['behandelingwww.bloemenhove.nl', 'Bloemenhovewww.bloemenhove.nl', 'Thuisartswww.thuisarts.nl', 'Trouwwww.trouw.nl', 'www.gezondheidsplein.nl', 'Fiomfiom.nl', 'www.telegraaf.nl', 'www.telegraaf.nl', 'Levenwww.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>['Rijksoverheidwww.rijksoverheid.nl', 'WURwww.wur.nl', 'www.clo.nl', 'Commissionec.europa.eu', 'Klimaat.bewww.klimaat.be', 'www.urgenda.nl', 'Milieudefensiemilieudefensie.nl', 'www.knaw.nl', 'HIERwww.hier.nu']</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>['Adwww.ad.nl', 'www.ad.nl', 'Volkskrantwww.volkskrant.nl', 'www.trouw.nl', 'www.nu.nl', 'NRCwww.nrc.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'nos.nl']</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>['Rijksvaccinatieprogramma.nlrijksvaccinatieprogramma.nl', 'Vaccinvrijstichtingvaccinvrij.nl', 'WantToKnowwww.wanttoknow.nl', 'gevolgen?www.nvkp.nl', 'meer!www.thuisvaccinatie.nl', 'Scientiaswww.scientias.nl', 'Utrechtwww.umcutrecht.nl', 'kindercoachwww.nieuwetijds-kindercoach.nl', 'vaccinerendekennisvannu.nl', 'GGDREISVACCINATIESwww.ggdreisvaccinaties.nl']</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>['Wikipedianl.wikipedia.org', 'Rijksoverheid.nlwww.rijksoverheid.nl', 'politie.nlwww.politie.nl', 'www.volkskrant.nl', 'decorrespondent.nl', 'uitgeprocedeerdenwww.amnesty.nl', 'decentraaleuropadecentraal.nl', 'www.elsevierweekblad.nl', 'Jaltajalta.nl', 'EUR-Lexeur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr"/>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>['behandelingwww.bloemenhove.nl', 'Bloemenhovewww.bloemenhove.nl', 'Thuisartswww.thuisarts.nl', 'Trouwwww.trouw.nl', 'www.gezondheidsplein.nl', 'Fiomfiom.nl', 'www.telegraaf.nl', 'www.telegraaf.nl', 'Levenwww.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>['Rijksoverheidwww.rijksoverheid.nl', 'WURwww.wur.nl', 'www.clo.nl', 'Commissionec.europa.eu', 'Klimaat.bewww.klimaat.be', 'www.urgenda.nl', 'Milieudefensiemilieudefensie.nl', 'www.knaw.nl', 'HIERwww.hier.nu']</t>
+        </is>
+      </c>
       <c r="D47" t="inlineStr">
         <is>
           <t>['Adwww.ad.nl', 'Volkskrantwww.volkskrant.nl', 'www.trouw.nl', 'www.nu.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'nos.nl', 'NRCwww.nrc.nl']</t>
         </is>
       </c>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>['Rijksvaccinatieprogramma.nlrijksvaccinatieprogramma.nl', 'Vaccinvrijstichtingvaccinvrij.nl', 'WantToKnowwww.wanttoknow.nl', 'gevolgen?www.nvkp.nl', 'meer!www.thuisvaccinatie.nl', 'Scientiaswww.scientias.nl', 'Utrechtwww.umcutrecht.nl', 'kindercoachwww.nieuwetijds-kindercoach.nl', 'vaccinerendekennisvannu.nl', 'GGDREISVACCINATIESwww.ggdreisvaccinaties.nl']</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>['Wikipedianl.wikipedia.org', 'Rijksoverheid.nlwww.rijksoverheid.nl', 'politie.nlwww.politie.nl', 'www.volkskrant.nl', 'decorrespondent.nl', 'uitgeprocedeerdenwww.amnesty.nl', 'decentraaleuropadecentraal.nl', 'www.elsevierweekblad.nl', 'Jaltajalta.nl', 'EUR-Lexeur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="B48" t="inlineStr"/>
-      <c r="C48" t="inlineStr"/>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>['behandelingwww.bloemenhove.nl', 'Bloemenhovewww.bloemenhove.nl', 'Thuisartswww.thuisarts.nl', 'Trouwwww.trouw.nl', 'www.gezondheidsplein.nl', 'Fiomfiom.nl', 'www.telegraaf.nl', 'Levenwww.schreeuwomleven.nl', 'Sense.infosense.info']</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>['Rijksoverheidwww.rijksoverheid.nl', 'WURwww.wur.nl', 'www.clo.nl', 'Commissionec.europa.eu', 'Klimaat.bewww.klimaat.be', 'www.urgenda.nl', 'Milieudefensiemilieudefensie.nl', 'www.knaw.nl', 'HIERwww.hier.nu']</t>
+        </is>
+      </c>
       <c r="D48" t="inlineStr">
         <is>
           <t>['Adwww.ad.nl', 'Volkskrantwww.volkskrant.nl', 'www.trouw.nl', 'www.nu.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'nos.nl', 'NRCwww.nrc.nl']</t>
         </is>
       </c>
-      <c r="E48" t="inlineStr"/>
-      <c r="F48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>['Rijksvaccinatieprogramma.nlrijksvaccinatieprogramma.nl', 'Vaccinvrijstichtingvaccinvrij.nl', 'WantToKnowwww.wanttoknow.nl', 'gevolgen?www.nvkp.nl', 'meer!www.thuisvaccinatie.nl', 'Scientiaswww.scientias.nl', 'Utrechtwww.umcutrecht.nl', 'kindercoachwww.nieuwetijds-kindercoach.nl', 'GGDREISVACCINATIESwww.ggdreisvaccinaties.nl', 'vaccinerendekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>['Wikipedianl.wikipedia.org', 'Rijksoverheid.nlwww.rijksoverheid.nl', 'politie.nlwww.politie.nl', 'www.volkskrant.nl', 'decorrespondent.nl', 'uitgeprocedeerdenwww.amnesty.nl', 'decentraaleuropadecentraal.nl', 'Jaltajalta.nl', 'www.elsevierweekblad.nl', 'EUR-Lexeur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49" t="inlineStr"/>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
-      <c r="F49" t="inlineStr"/>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>['behandelingwww.bloemenhove.nl', 'Bloemenhovewww.bloemenhove.nl', 'www.gezondheidsplein.nl', 'Thuisartswww.thuisarts.nl', 'Trouwwww.trouw.nl', 'Fiomfiom.nl', 'www.telegraaf.nl', 'AD.nlwww.ad.nl', 'Levenwww.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>['WURwww.wur.nl', 'Rijksoverheidwww.rijksoverheid.nl', 'HIERwww.hier.nu', 'Delftwww.ce.nl', 'Climategatewww.climategate.nl', 'Klimaat.bewww.klimaat.be', 'Energievergelijkwww.energievergelijk.nl', 'www.knaw.nl', 'www.urgenda.nl']</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>['Adwww.ad.nl', 'www.ad.nl', 'Volkskrantwww.volkskrant.nl', 'www.trouw.nl', 'www.nu.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'nos.nl', 'NRCwww.nrc.nl']</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>['Rijksvaccinatieprogramma.nlrijksvaccinatieprogramma.nl', 'WantToKnowwww.wanttoknow.nl', 'Vaccinvrijstichtingvaccinvrij.nl', 'gevolgen?www.nvkp.nl', 'meer!www.thuisvaccinatie.nl', 'Scientiaswww.scientias.nl', 'vaccinerenwww.laatjevaccineren.be', 'Diversenmens-en-gezondheid.infonu.nl', 'www.volkskrant.nl', 'Utrechtwww.umcutrecht.nl']</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>['Wikipedianl.wikipedia.org', 'Rijksoverheid.nlwww.rijksoverheid.nl', 'politie.nlwww.politie.nl', 'uitgeprocedeerdenwww.amnesty.nl', 'decentraaleuropadecentraal.nl', 'decorrespondent.nl', 'www.volkskrant.nl', 'www.volkskrant.nl', 'INDind.nl', 'EUR-Lexeur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr"/>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>['behandelingwww.bloemenhove.nl', 'Bloemenhovewww.bloemenhove.nl', 'www.gezondheidsplein.nl', 'Thuisartswww.thuisarts.nl', 'Trouwwww.trouw.nl', 'Fiomfiom.nl', 'www.telegraaf.nl', 'AD.nlwww.ad.nl', 'Levenwww.schreeuwomleven.nl']</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>['Rijksoverheidwww.rijksoverheid.nl', 'WURwww.wur.nl', 'www.clo.nl', 'Commissionec.europa.eu', 'Klimaat.bewww.klimaat.be', 'www.urgenda.nl', 'Milieudefensiemilieudefensie.nl', 'www.knaw.nl', 'HIERwww.hier.nu']</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>['Adwww.ad.nl', 'www.ad.nl', 'Volkskrantwww.volkskrant.nl', 'www.trouw.nl', 'www.nu.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'NRCwww.nrc.nl', 'nos.nl']</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>['Rijksvaccinatieprogramma.nlrijksvaccinatieprogramma.nl', 'Vaccinvrijstichtingvaccinvrij.nl', 'WantToKnowwww.wanttoknow.nl', 'gevolgen?www.nvkp.nl', 'meer!www.thuisvaccinatie.nl', 'Scientiaswww.scientias.nl', 'Utrechtwww.umcutrecht.nl', 'kindercoachwww.nieuwetijds-kindercoach.nl', 'www.volkskrant.nl', 'vaccinerendekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>['Wikipedianl.wikipedia.org', 'Rijksoverheid.nlwww.rijksoverheid.nl', 'politie.nlwww.politie.nl', 'www.volkskrant.nl', 'decorrespondent.nl', 'uitgeprocedeerdenwww.amnesty.nl', 'decentraaleuropadecentraal.nl', 'www.elsevierweekblad.nl', 'Jaltajalta.nl', 'EUR-Lexeur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>['behandelingwww.bloemenhove.nl', 'Thuisartswww.thuisarts.nl', 'Trouwwww.trouw.nl', 'www.gezondheidsplein.nl', 'Fiomfiom.nl', 'www.telegraaf.nl', 'Levenwww.schreeuwomleven.nl', 'Sense.infosense.info', 'AD.nlwww.ad.nl']</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>['Rijksoverheidwww.rijksoverheid.nl', 'WURwww.wur.nl', 'www.clo.nl', 'Commissionec.europa.eu', 'www.urgenda.nl', 'Klimaat.bewww.klimaat.be', 'HIERwww.hier.nu', 'Milieudefensiemilieudefensie.nl', 'www.knaw.nl']</t>
+        </is>
+      </c>
       <c r="D51" t="inlineStr">
         <is>
           <t>['AD.nlwww.ad.nl', 'Volkskrantwww.volkskrant.nl', 'www.trouw.nl', 'NRCwww.nrc.nl', 'eenvandaag.avrotros.nl', 'eenvandaag.avrotros.nl', 'nos.nl', 'www.nu.nl']</t>
         </is>
       </c>
-      <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>['Rijksvaccinatieprogramma.nlrijksvaccinatieprogramma.nl', 'Vaccinvrijstichtingvaccinvrij.nl', 'WantToKnow.nlwww.wanttoknow.nl', 'gevolgen?www.nvkp.nl', 'meer!www.thuisvaccinatie.nl', 'Scientiaswww.scientias.nl', 'Utrechtwww.umcutrecht.nl', 'kindercoachwww.nieuwetijds-kindercoach.nl', 'GGDREISVACCINATIESwww.ggdreisvaccinaties.nl', 'vaccinerendekennisvannu.nl']</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>['Wikipedianl.wikipedia.org', 'Rijksoverheid.nlwww.rijksoverheid.nl', 'politie.nlwww.politie.nl', 'www.volkskrant.nl', 'uitgeprocedeerdenwww.amnesty.nl', 'decorrespondent.nl', 'decentraaleuropadecentraal.nl', 'Jaltajalta.nl', 'www.elsevierweekblad.nl', 'EUR-Lexeur-lex.europa.eu']</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>